<commit_message>
add file log, agrreate table
</commit_message>
<xml_diff>
--- a/Data Warehouse.xlsx
+++ b/Data Warehouse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace-Python\Data-Warehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F30629-7676-42EF-8DD2-930CA44140A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880B3C18-D61C-4A9C-848C-1918DAE14749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{59B2C3CB-7028-4F48-80D1-84E5AE089023}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="211">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>DECIMAL</t>
-  </si>
-  <si>
-    <t>VARCHAR</t>
   </si>
   <si>
     <t>Field name</t>
@@ -2875,7 +2872,7 @@
   <dimension ref="A5:AV71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2891,18 +2888,18 @@
     </row>
     <row r="6" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2910,13 +2907,13 @@
         <v>44</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2924,13 +2921,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2938,10 +2935,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>0</v>
@@ -2952,7 +2949,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>48</v>
@@ -2966,10 +2963,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>2</v>
@@ -2980,10 +2977,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>3</v>
@@ -2994,10 +2991,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>4</v>
@@ -3008,10 +3005,10 @@
         <v>6</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>5</v>
@@ -3022,10 +3019,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>6</v>
@@ -3036,10 +3033,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>7</v>
@@ -3050,10 +3047,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>43</v>
@@ -3064,10 +3061,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>8</v>
@@ -3078,10 +3075,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>9</v>
@@ -3092,7 +3089,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>46</v>
@@ -3106,10 +3103,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>11</v>
@@ -3120,7 +3117,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>46</v>
@@ -3134,10 +3131,10 @@
         <v>15</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>13</v>
@@ -3148,10 +3145,10 @@
         <v>16</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>14</v>
@@ -3162,10 +3159,10 @@
         <v>17</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>15</v>
@@ -3176,10 +3173,10 @@
         <v>18</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>16</v>
@@ -3190,10 +3187,10 @@
         <v>19</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>17</v>
@@ -3204,10 +3201,10 @@
         <v>20</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>18</v>
@@ -3218,7 +3215,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>46</v>
@@ -3232,10 +3229,10 @@
         <v>22</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>20</v>
@@ -3246,10 +3243,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>21</v>
@@ -3260,10 +3257,10 @@
         <v>24</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>22</v>
@@ -3274,10 +3271,10 @@
         <v>25</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>23</v>
@@ -3288,10 +3285,10 @@
         <v>26</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>24</v>
@@ -3302,10 +3299,10 @@
         <v>27</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>25</v>
@@ -3316,10 +3313,10 @@
         <v>28</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>26</v>
@@ -3330,10 +3327,10 @@
         <v>29</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>27</v>
@@ -3344,10 +3341,10 @@
         <v>30</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>28</v>
@@ -3358,10 +3355,10 @@
         <v>31</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>29</v>
@@ -3372,10 +3369,10 @@
         <v>32</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>30</v>
@@ -3386,10 +3383,10 @@
         <v>33</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>31</v>
@@ -3400,10 +3397,10 @@
         <v>34</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>32</v>
@@ -3414,10 +3411,10 @@
         <v>35</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>33</v>
@@ -3428,10 +3425,10 @@
         <v>36</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>34</v>
@@ -3442,10 +3439,10 @@
         <v>37</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>35</v>
@@ -3456,10 +3453,10 @@
         <v>38</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>36</v>
@@ -3470,16 +3467,16 @@
         <v>39</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>37</v>
       </c>
       <c r="AV50" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3487,10 +3484,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>38</v>
@@ -3501,10 +3498,10 @@
         <v>41</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>39</v>
@@ -3515,10 +3512,10 @@
         <v>42</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>40</v>
@@ -3529,7 +3526,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>47</v>
@@ -3543,10 +3540,10 @@
         <v>44</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>42</v>
@@ -3557,13 +3554,13 @@
         <v>45</v>
       </c>
       <c r="B56" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3603,273 +3600,273 @@
     <row r="1" spans="1:45" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
       <c r="B1" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="S1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="U1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="V1" s="22" t="s">
+      <c r="W1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="Y1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="AA1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AC1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="AD1" s="22" t="s">
+      <c r="AE1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AG1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="AH1" s="22" t="s">
+      <c r="AI1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="AJ1" s="22" t="s">
+      <c r="AK1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="AL1" s="22" t="s">
+      <c r="AM1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="AN1" s="22" t="s">
+      <c r="AO1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="AP1" s="22" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="AR1" s="22" t="s">
+      <c r="AS1" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="T2" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="X2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="Y2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Z2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="AA2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AB2" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="13" t="s">
+      <c r="AC2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AC2" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AE2" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="AE2" s="13" t="s">
+      <c r="AF2" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AG2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="AG2" s="13" t="s">
+      <c r="AH2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="AH2" s="13" t="s">
+      <c r="AI2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="AI2" s="13" t="s">
+      <c r="AJ2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="AJ2" s="13" t="s">
+      <c r="AK2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="AK2" s="13" t="s">
+      <c r="AL2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="AL2" s="13" t="s">
+      <c r="AM2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AM2" s="13" t="s">
+      <c r="AN2" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="AN2" s="13" t="s">
+      <c r="AO2" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="AO2" s="13" t="s">
+      <c r="AP2" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="AP2" s="13" t="s">
+      <c r="AQ2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="AR2" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="AQ2" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="AR2" s="13" t="s">
+      <c r="AS2" s="15" t="s">
         <v>91</v>
-      </c>
-      <c r="AS2" s="15" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:45" ht="409.5" x14ac:dyDescent="0.25">
@@ -3877,136 +3874,136 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="AD3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AL3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AM3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AO3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AP3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="AR3" s="16">
         <v>45901</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:45" ht="409.5" x14ac:dyDescent="0.25">
@@ -4014,136 +4011,136 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AQ4" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="AR4" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS4" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:45" ht="409.5" x14ac:dyDescent="0.25">
@@ -4151,136 +4148,136 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="U5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="AR5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS5" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="AS5" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>